<commit_message>
Add experiment 12 notebook run in colab and its outputs (this time really using the sampler)
</commit_message>
<xml_diff>
--- a/experiments/experiment_12/outputs/train_results.xlsx
+++ b/experiments/experiment_12/outputs/train_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,34 +490,34 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3572890551930124</v>
+        <v>0.3932745998555964</v>
       </c>
       <c r="C2" t="n">
-        <v>0.027818024441329</v>
+        <v>0.1408304948214087</v>
       </c>
       <c r="D2" t="n">
-        <v>0.07880865425578502</v>
+        <v>0.1685173979717599</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5970043668268079</v>
+        <v>0.7391293804618444</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2345436818413073</v>
+        <v>0.3494924244183377</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3437324816530401</v>
+        <v>0.3857745582407171</v>
       </c>
       <c r="H2" t="n">
-        <v>0.06712244773144718</v>
+        <v>0.2137194715956052</v>
       </c>
       <c r="I2" t="n">
-        <v>0.153223338490889</v>
+        <v>0.08554073251665753</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6366143116232106</v>
+        <v>0.6259648642665308</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2856533659485156</v>
+        <v>0.3084083561262645</v>
       </c>
     </row>
     <row r="3">
@@ -525,34 +525,34 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3025324226103046</v>
+        <v>0.3006536300209435</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1462706651357162</v>
+        <v>0.3319560029834158</v>
       </c>
       <c r="D3" t="n">
-        <v>0.237398806056587</v>
+        <v>0.3629892125135751</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7316774905401654</v>
+        <v>0.8929213424302891</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3717823205774895</v>
+        <v>0.5292888526424266</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3313197303902019</v>
+        <v>0.3799167966300791</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1756029627550472</v>
+        <v>0.2563515613248645</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2308603266557991</v>
+        <v>0.1357430017761613</v>
       </c>
       <c r="J3" t="n">
-        <v>0.6571095132895591</v>
+        <v>0.6504452008466342</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3545242675668018</v>
+        <v>0.3475132546492199</v>
       </c>
     </row>
     <row r="4">
@@ -560,34 +560,34 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2834797513417222</v>
+        <v>0.2720153485848145</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2292116751423338</v>
+        <v>0.4458851715843121</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3289249239777515</v>
+        <v>0.4844337668685518</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7829323253923242</v>
+        <v>0.9139438758543744</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4470229748374698</v>
+        <v>0.614754271435746</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3244060413403945</v>
+        <v>0.3647804355079478</v>
       </c>
       <c r="H4" t="n">
-        <v>0.203495004559105</v>
+        <v>0.2613958985206534</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2640144700121411</v>
+        <v>0.1454856550393352</v>
       </c>
       <c r="J4" t="n">
-        <v>0.6689673803663312</v>
+        <v>0.6618481730766624</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3788256183125258</v>
+        <v>0.356243242212217</v>
       </c>
     </row>
     <row r="5">
@@ -595,34 +595,34 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2697804079137065</v>
+        <v>0.2438839638436383</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2679414043259211</v>
+        <v>0.5276052950528571</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3788471730707524</v>
+        <v>0.5680182163517489</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8162625976279989</v>
+        <v>0.9355454375974959</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4876837250082242</v>
+        <v>0.677056316334034</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3200536261905323</v>
+        <v>0.3700670112263073</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2099409352993953</v>
+        <v>0.2730910161460464</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2715912750295865</v>
+        <v>0.1734839728854123</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6760454083320815</v>
+        <v>0.6620320364465969</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3858592062203544</v>
+        <v>0.3695356751593519</v>
       </c>
     </row>
     <row r="6">
@@ -630,34 +630,34 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2587526364421303</v>
+        <v>0.2283100086179647</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3006334489103973</v>
+        <v>0.5976626517887789</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4289748659415498</v>
+        <v>0.6361537972613508</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8402614275954751</v>
+        <v>0.9431363723664695</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5232899141491407</v>
+        <v>0.7256509404721997</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3170923116532239</v>
+        <v>0.369258238510652</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2166723701083998</v>
+        <v>0.2985968985051409</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2819156657071928</v>
+        <v>0.1892949958312445</v>
       </c>
       <c r="J6" t="n">
-        <v>0.6811133541154736</v>
+        <v>0.6605657260535066</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3932337966436887</v>
+        <v>0.3828192067966307</v>
       </c>
     </row>
     <row r="7">
@@ -665,34 +665,34 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2494235387579961</v>
+        <v>0.212736055593599</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3238216720776662</v>
+        <v>0.6529513027178655</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4641721563058293</v>
+        <v>0.6915876685279339</v>
       </c>
       <c r="E7" t="n">
-        <v>0.858608899818752</v>
+        <v>0.9550285543023033</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5488675760674159</v>
+        <v>0.7665225085160342</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3149905855005438</v>
+        <v>0.3634841916236011</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2176801016706576</v>
+        <v>0.2886340387049195</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2861616150527018</v>
+        <v>0.1993230298643209</v>
       </c>
       <c r="J7" t="n">
-        <v>0.6843231017189145</v>
+        <v>0.6663832959088419</v>
       </c>
       <c r="K7" t="n">
-        <v>0.396054939480758</v>
+        <v>0.3847801214926941</v>
       </c>
     </row>
     <row r="8">
@@ -700,34 +700,34 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2413055331192233</v>
+        <v>0.2015304379165173</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3390792024086835</v>
+        <v>0.6771687612751056</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4848735365144974</v>
+        <v>0.7136951935294482</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8731549908478187</v>
+        <v>0.9619346365568585</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5657025765903332</v>
+        <v>0.7842661971204707</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3134610178795728</v>
+        <v>0.3653716228225015</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2182553107588628</v>
+        <v>0.3105390539763141</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2925592687427233</v>
+        <v>0.2188414312398663</v>
       </c>
       <c r="J8" t="n">
-        <v>0.6865272459029632</v>
+        <v>0.6676084129199261</v>
       </c>
       <c r="K8" t="n">
-        <v>0.3991139418015164</v>
+        <v>0.3989962993787022</v>
       </c>
     </row>
     <row r="9">
@@ -735,34 +735,34 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2341093940829689</v>
+        <v>0.1952455917542631</v>
       </c>
       <c r="C9" t="n">
-        <v>0.365535212504624</v>
+        <v>0.709098847254658</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5149490443753094</v>
+        <v>0.7443457663057985</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8851264279884381</v>
+        <v>0.9610586005919607</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5885368949561238</v>
+        <v>0.8048344047174724</v>
       </c>
       <c r="G9" t="n">
-        <v>0.312330733646046</v>
+        <v>0.3667589642784812</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2144160248079027</v>
+        <v>0.3042006831659118</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2939003835466673</v>
+        <v>0.2196759252029084</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6878538417282001</v>
+        <v>0.668531465661066</v>
       </c>
       <c r="K9" t="n">
-        <v>0.3987234166942566</v>
+        <v>0.397469358009962</v>
       </c>
     </row>
     <row r="10">
@@ -770,34 +770,34 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2276457566767931</v>
+        <v>0.1862227354537357</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3833030370803155</v>
+        <v>0.7252423121675486</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5334978258516877</v>
+        <v>0.7591362309917017</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8952022264812648</v>
+        <v>0.9657979803548533</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6040010298044227</v>
+        <v>0.8167255078380347</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3114879781549627</v>
+        <v>0.3601538796316494</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2158578910539349</v>
+        <v>0.3067095084392863</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2991958312769077</v>
+        <v>0.2348047726859173</v>
       </c>
       <c r="J10" t="n">
-        <v>0.6884250389268191</v>
+        <v>0.6688423451513434</v>
       </c>
       <c r="K10" t="n">
-        <v>0.4011595870858873</v>
+        <v>0.403452208758849</v>
       </c>
     </row>
     <row r="11">
@@ -805,34 +805,34 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2217825415798209</v>
+        <v>0.1800986508076841</v>
       </c>
       <c r="C11" t="n">
-        <v>0.404634054386302</v>
+        <v>0.7358239760720542</v>
       </c>
       <c r="D11" t="n">
-        <v>0.55566861251642</v>
+        <v>0.7687943334624554</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9038322770152508</v>
+        <v>0.9653786486243032</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6213783146393242</v>
+        <v>0.8233323193862709</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3108567771586505</v>
+        <v>0.3476156687194651</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2161897022665709</v>
+        <v>0.3073065722378538</v>
       </c>
       <c r="I11" t="n">
-        <v>0.3015511645680015</v>
+        <v>0.2493648624783918</v>
       </c>
       <c r="J11" t="n">
-        <v>0.6889561792052781</v>
+        <v>0.6712514134921433</v>
       </c>
       <c r="K11" t="n">
-        <v>0.4022323486799501</v>
+        <v>0.4093076160694629</v>
       </c>
     </row>
     <row r="12">
@@ -840,34 +840,34 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2164234806868163</v>
+        <v>0.1684191976250573</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4216550082593903</v>
+        <v>0.7771058007899558</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5737624288584968</v>
+        <v>0.8061519437791798</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9113057414008157</v>
+        <v>0.9721495505552318</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6355743928395676</v>
+        <v>0.8518024317081224</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3103838752616536</v>
+        <v>0.3540679243477908</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2092312670630323</v>
+        <v>0.3207794056052277</v>
       </c>
       <c r="I12" t="n">
-        <v>0.300608580692994</v>
+        <v>0.2591921951600958</v>
       </c>
       <c r="J12" t="n">
-        <v>0.6894123659650538</v>
+        <v>0.6742976545498321</v>
       </c>
       <c r="K12" t="n">
-        <v>0.3997507379070267</v>
+        <v>0.4180897517717185</v>
       </c>
     </row>
     <row r="13">
@@ -875,34 +875,34 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.211496085351841</v>
+        <v>0.1640105035833337</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4396395444041304</v>
+        <v>0.7880044465718756</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5942036652211525</v>
+        <v>0.8159500516734347</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9178619148934715</v>
+        <v>0.973496468683847</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6505683748395849</v>
+        <v>0.859150322309719</v>
       </c>
       <c r="G13" t="n">
-        <v>0.3100312663750215</v>
+        <v>0.3579143353483893</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2223141313734075</v>
+        <v>0.3127294769675363</v>
       </c>
       <c r="I13" t="n">
-        <v>0.3095782968641378</v>
+        <v>0.2521654263488198</v>
       </c>
       <c r="J13" t="n">
-        <v>0.689637061713184</v>
+        <v>0.6712505904120487</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4071764966502431</v>
+        <v>0.4120484979094683</v>
       </c>
     </row>
     <row r="14">
@@ -910,34 +910,34 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2069442794573578</v>
+        <v>0.1630469653755426</v>
       </c>
       <c r="C14" t="n">
-        <v>0.455652321478085</v>
+        <v>0.7778694234918657</v>
       </c>
       <c r="D14" t="n">
-        <v>0.610054597241147</v>
+        <v>0.8067193939534946</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9235696768422952</v>
+        <v>0.9724847127586883</v>
       </c>
       <c r="F14" t="n">
-        <v>0.663092198520509</v>
+        <v>0.8523578434013496</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3097717816179449</v>
+        <v>0.3567676923491738</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2250667885229057</v>
+        <v>0.3122298973747675</v>
       </c>
       <c r="I14" t="n">
-        <v>0.3116989597872939</v>
+        <v>0.2444950772789654</v>
       </c>
       <c r="J14" t="n">
-        <v>0.6898131913921257</v>
+        <v>0.6748432834038122</v>
       </c>
       <c r="K14" t="n">
-        <v>0.4088596465674418</v>
+        <v>0.4105227526858484</v>
       </c>
     </row>
     <row r="15">
@@ -945,34 +945,34 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2027236753228036</v>
+        <v>0.1555034209212119</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4682843612964628</v>
+        <v>0.8042110555983735</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6224428266686929</v>
+        <v>0.8314296510608431</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9286929275598778</v>
+        <v>0.9757179814084243</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6731400385083445</v>
+        <v>0.8704528960225469</v>
       </c>
       <c r="G15" t="n">
-        <v>0.3095859546553005</v>
+        <v>0.3546480292623693</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2269421541531459</v>
+        <v>0.3212374474091687</v>
       </c>
       <c r="I15" t="n">
-        <v>0.3124828350422951</v>
+        <v>0.2914322291938585</v>
       </c>
       <c r="J15" t="n">
-        <v>0.6897979422786856</v>
+        <v>0.6769060708167497</v>
       </c>
       <c r="K15" t="n">
-        <v>0.4097409771580423</v>
+        <v>0.429858582473259</v>
       </c>
     </row>
     <row r="16">
@@ -980,34 +980,34 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1987983586097306</v>
+        <v>0.1522287286987359</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4783068040571095</v>
+        <v>0.8134133823534728</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6359591039795964</v>
+        <v>0.8394621948930137</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9332243327089181</v>
+        <v>0.9759292924108572</v>
       </c>
       <c r="F16" t="n">
-        <v>0.682496746915208</v>
+        <v>0.8762682898857812</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3094598420641639</v>
+        <v>0.3523896038532257</v>
       </c>
       <c r="H16" t="n">
-        <v>0.2281761985910175</v>
+        <v>0.3096303347638837</v>
       </c>
       <c r="I16" t="n">
-        <v>0.3157403602079602</v>
+        <v>0.2761703147715955</v>
       </c>
       <c r="J16" t="n">
-        <v>0.6895334678030139</v>
+        <v>0.6747427349052497</v>
       </c>
       <c r="K16" t="n">
-        <v>0.4111500088673306</v>
+        <v>0.4201811281469096</v>
       </c>
     </row>
     <row r="17">
@@ -1015,34 +1015,34 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.195138669742102</v>
+        <v>0.1482766097072851</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4900592793832721</v>
+        <v>0.8235098632704061</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6488141889360524</v>
+        <v>0.8480039546023116</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9372607677869521</v>
+        <v>0.9759707789278126</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6920447453687588</v>
+        <v>0.8824948656001768</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3093832975084131</v>
+        <v>0.3538659052415328</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2263818985753581</v>
+        <v>0.3132373783376345</v>
       </c>
       <c r="I17" t="n">
-        <v>0.3146377269684503</v>
+        <v>0.2648189900150066</v>
       </c>
       <c r="J17" t="n">
-        <v>0.6893328810443182</v>
+        <v>0.6739434229892358</v>
       </c>
       <c r="K17" t="n">
-        <v>0.4101175021960422</v>
+        <v>0.4173332637806257</v>
       </c>
     </row>
     <row r="18">
@@ -1050,34 +1050,34 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1917196446183053</v>
+        <v>0.1455070046199994</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5002412033686212</v>
+        <v>0.8225826223986079</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6572452804991331</v>
+        <v>0.8463740235406541</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9409437259960944</v>
+        <v>0.9759659239121411</v>
       </c>
       <c r="F18" t="n">
-        <v>0.6994767366212828</v>
+        <v>0.8816408566171344</v>
       </c>
       <c r="G18" t="n">
-        <v>0.3093487159772353</v>
+        <v>0.3561408465558832</v>
       </c>
       <c r="H18" t="n">
-        <v>0.2259121863730751</v>
+        <v>0.3138169111922792</v>
       </c>
       <c r="I18" t="n">
-        <v>0.3150845692248905</v>
+        <v>0.2664505925128974</v>
       </c>
       <c r="J18" t="n">
-        <v>0.6891226925806895</v>
+        <v>0.671019271459646</v>
       </c>
       <c r="K18" t="n">
-        <v>0.4100398160595517</v>
+        <v>0.4170955917216075</v>
       </c>
     </row>
     <row r="19">
@@ -1085,34 +1085,34 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1885199192911386</v>
+        <v>0.1414309634234417</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5183891382337507</v>
+        <v>0.838925545663512</v>
       </c>
       <c r="D19" t="n">
-        <v>0.668405663651491</v>
+        <v>0.8616727481562716</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9442641038190016</v>
+        <v>0.9776281710418845</v>
       </c>
       <c r="F19" t="n">
-        <v>0.7103529685680812</v>
+        <v>0.8927421549538893</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3093501491980119</v>
+        <v>0.356943360783837</v>
       </c>
       <c r="H19" t="n">
-        <v>0.226088634012771</v>
+        <v>0.3060873034965687</v>
       </c>
       <c r="I19" t="n">
-        <v>0.3167652087898316</v>
+        <v>0.2607880489251808</v>
       </c>
       <c r="J19" t="n">
-        <v>0.6888871862892982</v>
+        <v>0.6686477251033506</v>
       </c>
       <c r="K19" t="n">
-        <v>0.4105803430306336</v>
+        <v>0.4118410258417</v>
       </c>
     </row>
     <row r="20">
@@ -1120,34 +1120,34 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1855209588327191</v>
+        <v>0.1418963412500241</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5316551878403255</v>
+        <v>0.8328249038650868</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6789422531083382</v>
+        <v>0.8562350474637105</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9471845134475817</v>
+        <v>0.9772646996377454</v>
       </c>
       <c r="F20" t="n">
-        <v>0.7192606514654152</v>
+        <v>0.8887748836555143</v>
       </c>
       <c r="G20" t="n">
-        <v>0.3093827664852142</v>
+        <v>0.3511937707662582</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2254828294881003</v>
+        <v>0.3198694583523346</v>
       </c>
       <c r="I20" t="n">
-        <v>0.3172312854959976</v>
+        <v>0.2823080012107084</v>
       </c>
       <c r="J20" t="n">
-        <v>0.6887142630238616</v>
+        <v>0.6696678000530285</v>
       </c>
       <c r="K20" t="n">
-        <v>0.4104761260026532</v>
+        <v>0.4239484198720238</v>
       </c>
     </row>
     <row r="21">
@@ -1155,34 +1155,34 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1827065033668822</v>
+        <v>0.1419485839591785</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5430068879226357</v>
+        <v>0.8310488437242581</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6865979465176499</v>
+        <v>0.8545901225939636</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9498988408796759</v>
+        <v>0.9770043938291986</v>
       </c>
       <c r="F21" t="n">
-        <v>0.7265012251066539</v>
+        <v>0.8875477867158068</v>
       </c>
       <c r="G21" t="n">
-        <v>0.3094424551183527</v>
+        <v>0.3544465452432632</v>
       </c>
       <c r="H21" t="n">
-        <v>0.2283311361533641</v>
+        <v>0.3229854020092471</v>
       </c>
       <c r="I21" t="n">
-        <v>0.3183694908896498</v>
+        <v>0.2907355351084071</v>
       </c>
       <c r="J21" t="n">
-        <v>0.6886834398563315</v>
+        <v>0.6767913581258402</v>
       </c>
       <c r="K21" t="n">
-        <v>0.4117946889664485</v>
+        <v>0.4301707650811648</v>
       </c>
     </row>
     <row r="22">
@@ -1190,34 +1190,34 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1800621734424071</v>
+        <v>0.1382791675965894</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5545848525162658</v>
+        <v>0.8474769161130664</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6967845693240465</v>
+        <v>0.8690741042174516</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9523963155278149</v>
+        <v>0.9772544862138336</v>
       </c>
       <c r="F22" t="n">
-        <v>0.734588579122709</v>
+        <v>0.8979351688481172</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3095257404175671</v>
+        <v>0.3556863110173832</v>
       </c>
       <c r="H22" t="n">
-        <v>0.2323064411475474</v>
+        <v>0.3025445740788557</v>
       </c>
       <c r="I22" t="n">
-        <v>0.3229201954361105</v>
+        <v>0.2825430301185435</v>
       </c>
       <c r="J22" t="n">
-        <v>0.6884209249757338</v>
+        <v>0.6718770151181109</v>
       </c>
       <c r="K22" t="n">
-        <v>0.4145491871864639</v>
+        <v>0.4189882064385033</v>
       </c>
     </row>
     <row r="23">
@@ -1225,34 +1225,34 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1775751641358841</v>
+        <v>0.1340966998514804</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5638212019443669</v>
+        <v>0.8488053884462227</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7069797223120584</v>
+        <v>0.8705296340918551</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9545611643190345</v>
+        <v>0.980597054582388</v>
       </c>
       <c r="F23" t="n">
-        <v>0.7417873628584867</v>
+        <v>0.8999773590401552</v>
       </c>
       <c r="G23" t="n">
-        <v>0.3096295947378332</v>
+        <v>0.3550498214634982</v>
       </c>
       <c r="H23" t="n">
-        <v>0.2350358358961407</v>
+        <v>0.315313363295408</v>
       </c>
       <c r="I23" t="n">
-        <v>0.3306685155568701</v>
+        <v>0.2591009451058928</v>
       </c>
       <c r="J23" t="n">
-        <v>0.6882332162674839</v>
+        <v>0.6779356435432977</v>
       </c>
       <c r="K23" t="n">
-        <v>0.4179791892401649</v>
+        <v>0.4174499839815328</v>
       </c>
     </row>
     <row r="24">
@@ -1260,34 +1260,34 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.175234025513584</v>
+        <v>0.1325043359432708</v>
       </c>
       <c r="C24" t="n">
-        <v>0.5693974714514223</v>
+        <v>0.8565450897552058</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7126760983722701</v>
+        <v>0.8774461375221525</v>
       </c>
       <c r="E24" t="n">
-        <v>0.956605930977029</v>
+        <v>0.9785200907741115</v>
       </c>
       <c r="F24" t="n">
-        <v>0.7462265002669071</v>
+        <v>0.9041704393504899</v>
       </c>
       <c r="G24" t="n">
-        <v>0.3097514713352377</v>
+        <v>0.3546180657365106</v>
       </c>
       <c r="H24" t="n">
-        <v>0.2316057727755796</v>
+        <v>0.3173574182773939</v>
       </c>
       <c r="I24" t="n">
-        <v>0.3260672345022138</v>
+        <v>0.2826761652005808</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6879573319578045</v>
+        <v>0.6710912685529616</v>
       </c>
       <c r="K24" t="n">
-        <v>0.4152101130785327</v>
+        <v>0.4237082840103121</v>
       </c>
     </row>
     <row r="25">
@@ -1295,34 +1295,34 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.1730284772135995</v>
+        <v>0.130618718622083</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5763363183721584</v>
+        <v>0.8577814771578021</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7185863458571314</v>
+        <v>0.8784401219372651</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9584595664083717</v>
+        <v>0.9806551660451386</v>
       </c>
       <c r="F25" t="n">
-        <v>0.7511274102125539</v>
+        <v>0.9056255883800685</v>
       </c>
       <c r="G25" t="n">
-        <v>0.3098892197012901</v>
+        <v>0.3605144037441774</v>
       </c>
       <c r="H25" t="n">
-        <v>0.2370920787715149</v>
+        <v>0.3235320229028801</v>
       </c>
       <c r="I25" t="n">
-        <v>0.3292167671223808</v>
+        <v>0.2590952480321285</v>
       </c>
       <c r="J25" t="n">
-        <v>0.6877431815624893</v>
+        <v>0.6713130884880757</v>
       </c>
       <c r="K25" t="n">
-        <v>0.4180173424854617</v>
+        <v>0.4179801198076947</v>
       </c>
     </row>
     <row r="26">
@@ -1330,34 +1330,34 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1709492516449907</v>
+        <v>0.1256888574835929</v>
       </c>
       <c r="C26" t="n">
-        <v>0.5899247033179493</v>
+        <v>0.8691479461186709</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7270467723373999</v>
+        <v>0.8880260653158691</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9601311045812496</v>
+        <v>0.982474037970148</v>
       </c>
       <c r="F26" t="n">
-        <v>0.7590341934121997</v>
+        <v>0.9132160164682294</v>
       </c>
       <c r="G26" t="n">
-        <v>0.3100410449233922</v>
+        <v>0.3604879758574746</v>
       </c>
       <c r="H26" t="n">
-        <v>0.2368812502118888</v>
+        <v>0.3200581557682762</v>
       </c>
       <c r="I26" t="n">
-        <v>0.3307808891944262</v>
+        <v>0.2798961392243609</v>
       </c>
       <c r="J26" t="n">
-        <v>0.6875178642160908</v>
+        <v>0.6667484821254199</v>
       </c>
       <c r="K26" t="n">
-        <v>0.418393334540802</v>
+        <v>0.4222342590393524</v>
       </c>
     </row>
     <row r="27">
@@ -1365,34 +1365,34 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.1689879685978998</v>
+        <v>0.1254873500967568</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5964110841804739</v>
+        <v>0.8657727228843446</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7333482987429102</v>
+        <v>0.8856476400518855</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9616970923607564</v>
+        <v>0.982811122749512</v>
       </c>
       <c r="F27" t="n">
-        <v>0.7638188250947135</v>
+        <v>0.9114104952285805</v>
       </c>
       <c r="G27" t="n">
-        <v>0.3102054880423979</v>
+        <v>0.3600418811494654</v>
       </c>
       <c r="H27" t="n">
-        <v>0.2350563704942472</v>
+        <v>0.3070836603813325</v>
       </c>
       <c r="I27" t="n">
-        <v>0.3327314235750746</v>
+        <v>0.2788843218094756</v>
       </c>
       <c r="J27" t="n">
-        <v>0.6873051772056459</v>
+        <v>0.6684121012488613</v>
       </c>
       <c r="K27" t="n">
-        <v>0.4183643237583226</v>
+        <v>0.4181266944798898</v>
       </c>
     </row>
     <row r="28">
@@ -1400,34 +1400,34 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1671370389786634</v>
+        <v>0.1223351948640563</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6025855612470006</v>
+        <v>0.8741812531490297</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7386843048362703</v>
+        <v>0.8927806759597235</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9631718799978444</v>
+        <v>0.9832118883236679</v>
       </c>
       <c r="F28" t="n">
-        <v>0.7681472486937051</v>
+        <v>0.9167246058108071</v>
       </c>
       <c r="G28" t="n">
-        <v>0.310381296006116</v>
+        <v>0.3665613721717488</v>
       </c>
       <c r="H28" t="n">
-        <v>0.2269703492873739</v>
+        <v>0.327015023169232</v>
       </c>
       <c r="I28" t="n">
-        <v>0.3282389932870334</v>
+        <v>0.2852411647841827</v>
       </c>
       <c r="J28" t="n">
-        <v>0.6871061169914692</v>
+        <v>0.6743188220283848</v>
       </c>
       <c r="K28" t="n">
-        <v>0.4141051531886255</v>
+        <v>0.4288583366605998</v>
       </c>
     </row>
     <row r="29">
@@ -1435,34 +1435,34 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1653895801441236</v>
+        <v>0.1224568120457909</v>
       </c>
       <c r="C29" t="n">
-        <v>0.6097538265201815</v>
+        <v>0.8714612095906669</v>
       </c>
       <c r="D29" t="n">
-        <v>0.7442787430909026</v>
+        <v>0.8903870816018767</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9644914332103788</v>
+        <v>0.9838700298696704</v>
       </c>
       <c r="F29" t="n">
-        <v>0.7728413342738211</v>
+        <v>0.9152394403540712</v>
       </c>
       <c r="G29" t="n">
-        <v>0.3105673546140844</v>
+        <v>0.3610788217999719</v>
       </c>
       <c r="H29" t="n">
-        <v>0.2340791387467897</v>
+        <v>0.3278269920722423</v>
       </c>
       <c r="I29" t="n">
-        <v>0.3336789903218109</v>
+        <v>0.276955990289854</v>
       </c>
       <c r="J29" t="n">
-        <v>0.686962455242262</v>
+        <v>0.6723833818377015</v>
       </c>
       <c r="K29" t="n">
-        <v>0.4182401947702876</v>
+        <v>0.4257221213999325</v>
       </c>
     </row>
     <row r="30">
@@ -1470,34 +1470,34 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1637393439357931</v>
+        <v>0.1274335711178455</v>
       </c>
       <c r="C30" t="n">
-        <v>0.6181969862582312</v>
+        <v>0.8642023250716663</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7500343006195749</v>
+        <v>0.8839131660441072</v>
       </c>
       <c r="E30" t="n">
-        <v>0.9657262433712758</v>
+        <v>0.9792136875407693</v>
       </c>
       <c r="F30" t="n">
-        <v>0.7779858434163606</v>
+        <v>0.9091097262188477</v>
       </c>
       <c r="G30" t="n">
-        <v>0.310762574726885</v>
+        <v>0.3596594360741702</v>
       </c>
       <c r="H30" t="n">
-        <v>0.2357158788646387</v>
+        <v>0.3203660311347416</v>
       </c>
       <c r="I30" t="n">
-        <v>0.3361642198422878</v>
+        <v>0.2793323715843034</v>
       </c>
       <c r="J30" t="n">
-        <v>0.6868266763004727</v>
+        <v>0.674265904948625</v>
       </c>
       <c r="K30" t="n">
-        <v>0.4195689250024664</v>
+        <v>0.4246547692225567</v>
       </c>
     </row>
     <row r="31">
@@ -1505,279 +1505,34 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.1621806834909049</v>
+        <v>0.1223925907503475</v>
       </c>
       <c r="C31" t="n">
-        <v>0.6251016001457719</v>
+        <v>0.8747876246070937</v>
       </c>
       <c r="D31" t="n">
-        <v>0.7543157199612495</v>
+        <v>0.8935995829765024</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9668596933372671</v>
+        <v>0.9824003801562629</v>
       </c>
       <c r="F31" t="n">
-        <v>0.7820923378147628</v>
+        <v>0.9169291959132865</v>
       </c>
       <c r="G31" t="n">
-        <v>0.3109658191149885</v>
+        <v>0.3621440353718671</v>
       </c>
       <c r="H31" t="n">
-        <v>0.2338366943876379</v>
+        <v>0.3246390108023775</v>
       </c>
       <c r="I31" t="n">
-        <v>0.3352119339171768</v>
+        <v>0.2799716316101554</v>
       </c>
       <c r="J31" t="n">
-        <v>0.6866275390498756</v>
+        <v>0.6741453791895402</v>
       </c>
       <c r="K31" t="n">
-        <v>0.4185587224515634</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="n">
-        <v>0.1607084981250492</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0.6358681058431453</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.7616055378942781</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.9679539724791875</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0.7884758720722037</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0.3111757608977231</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.2338912621995903</v>
-      </c>
-      <c r="I32" t="n">
-        <v>0.336316916407695</v>
-      </c>
-      <c r="J32" t="n">
-        <v>0.6864638150264168</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0.4188906645445674</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="n">
-        <v>0.159318225288933</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0.6401022617502083</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.7645624292901843</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.9689437451151179</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0.791202812051837</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0.3113908456130461</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0.2338912621995903</v>
-      </c>
-      <c r="I33" t="n">
-        <v>0.336316916407695</v>
-      </c>
-      <c r="J33" t="n">
-        <v>0.6863106605006626</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0.4188396130359826</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="n">
-        <v>0.1580058004368435</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.6449018121801608</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.7685892679063575</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.9698731131572063</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0.7944547310812414</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0.3116092830896378</v>
-      </c>
-      <c r="H34" t="n">
-        <v>0.232482589757333</v>
-      </c>
-      <c r="I34" t="n">
-        <v>0.3371021495563004</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0.6861479069297097</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0.418577548747781</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="n">
-        <v>0.1567676413634961</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.6545203883630831</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.7750017348494228</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.9707355100408759</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0.8000858777511274</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0.3118290420282971</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0.2325247466341125</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0.3380834017851541</v>
-      </c>
-      <c r="J35" t="n">
-        <v>0.6860074281554192</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0.4188718588582286</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="n">
-        <v>0.1556006170470606</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0.6650250944803123</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0.7807291212523302</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.9715067909561252</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0.8057536688962559</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0.3120479190891439</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0.2327886528972328</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0.3389719453356375</v>
-      </c>
-      <c r="J36" t="n">
-        <v>0.6858193629119075</v>
-      </c>
-      <c r="K36" t="n">
-        <v>0.4191933203815926</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0.1545019992203875</v>
-      </c>
-      <c r="C37" t="n">
-        <v>0.668752778447065</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0.7831830006953711</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0.9722493455606289</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0.8080617082343551</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0.3122635768218474</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0.232163866767067</v>
-      </c>
-      <c r="I37" t="n">
-        <v>0.3384724779833921</v>
-      </c>
-      <c r="J37" t="n">
-        <v>0.6856965482305354</v>
-      </c>
-      <c r="K37" t="n">
-        <v>0.4187776309936648</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="n">
-        <v>0.1534694252874363</v>
-      </c>
-      <c r="C38" t="n">
-        <v>0.6767957864557197</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0.7876233992799657</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.9729394561880164</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0.812452880641234</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.312473631717942</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.2331593550364197</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0.3402075985866816</v>
-      </c>
-      <c r="J38" t="n">
-        <v>0.6855717023108087</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0.4196462186446366</v>
+        <v>0.426252007200691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>